<commit_message>
fixed the renaming code to handle duplicates
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -14,426 +14,1722 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="572">
+  <si>
+    <t>a01000.jpg</t>
+  </si>
+  <si>
+    <t>agb-fsmj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01002.jpg</t>
+  </si>
+  <si>
+    <t>agb-axvj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01004.jpg</t>
+  </si>
+  <si>
+    <t>agb-axvj-jpn-1.jpg</t>
+  </si>
+  <si>
+    <t>a01006.jpg</t>
+  </si>
+  <si>
+    <t>agb-bprj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01008.jpg</t>
+  </si>
+  <si>
+    <t>agb-axpj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01010.jpg</t>
+  </si>
+  <si>
+    <t>agb-axpj-jpn-2.jpg</t>
+  </si>
+  <si>
+    <t>a01012.jpg</t>
+  </si>
+  <si>
+    <t>agb-b4bj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01014.jpg</t>
+  </si>
+  <si>
+    <t>agb-a7kj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01016.jpg</t>
+  </si>
+  <si>
+    <t>agb-bsbj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01018.jpg</t>
+  </si>
+  <si>
+    <t>agb-asoj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01020.jpg</t>
+  </si>
+  <si>
+    <t>agb-brbj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01022.jpg</t>
+  </si>
+  <si>
+    <t>agb-br5j-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01024.jpg</t>
+  </si>
+  <si>
+    <t>agb-br5j-jpn-3.jpg</t>
+  </si>
+  <si>
+    <t>a01026.jpg</t>
+  </si>
+  <si>
+    <t>agb-a3gj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01028.jpg</t>
+  </si>
+  <si>
+    <t>agb-a9lj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01030.jpg</t>
+  </si>
+  <si>
+    <t>agb-ausj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01032.jpg</t>
+  </si>
+  <si>
+    <t>agb-a4gj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01034.jpg</t>
+  </si>
+  <si>
+    <t>agb-bnrj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01036.jpg</t>
+  </si>
+  <si>
+    <t>agb-amtj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01038.jpg</t>
+  </si>
+  <si>
+    <t>agb-arhj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01040.jpg</t>
+  </si>
+  <si>
+    <t>agb-amuj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01042.jpg</t>
+  </si>
+  <si>
+    <t>agb-bngj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01044.jpg</t>
+  </si>
+  <si>
+    <t>agb-azgj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01046.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ataj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01048.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ataj-jpn-4.jpg</t>
+  </si>
+  <si>
+    <t>a01050.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ataj-jpn-5.jpg</t>
+  </si>
+  <si>
+    <t>a01052.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ataj-jpn-6.jpg</t>
+  </si>
+  <si>
+    <t>a01054.jpg</t>
+  </si>
+  <si>
+    <t>dmg-at3j-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01056.jpg</t>
+  </si>
+  <si>
+    <t>dmg-at3j-jpn-7.jpg</t>
+  </si>
+  <si>
+    <t>a01058.jpg</t>
+  </si>
+  <si>
+    <t>dmg-at3j-jpn-8.jpg</t>
+  </si>
+  <si>
+    <t>a01060.jpg</t>
+  </si>
+  <si>
+    <t>dmg-at3j-jpn-9.jpg</t>
+  </si>
+  <si>
+    <t>a01062.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ytj.jpg</t>
+  </si>
+  <si>
+    <t>a01064.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ytj-10.jpg</t>
+  </si>
+  <si>
+    <t>a01066.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ytj-11.jpg</t>
+  </si>
+  <si>
+    <t>a01068.jpg</t>
+  </si>
+  <si>
+    <t>dmg-mla.jpg</t>
+  </si>
+  <si>
+    <t>a01070.jpg</t>
+  </si>
+  <si>
+    <t>dmg-mla-12.jpg</t>
+  </si>
+  <si>
+    <t>a01072.jpg</t>
+  </si>
+  <si>
+    <t>dmg-mla-13.jpg</t>
+  </si>
+  <si>
+    <t>a01074.jpg</t>
+  </si>
+  <si>
+    <t>dmg-mla-14.jpg</t>
+  </si>
+  <si>
+    <t>a01076.jpg</t>
+  </si>
+  <si>
+    <t>dmg-mla-15.jpg</t>
+  </si>
+  <si>
+    <t>a01078.jpg</t>
+  </si>
+  <si>
+    <t>dmg-mla-16.jpg</t>
+  </si>
+  <si>
+    <t>a01080.jpg</t>
+  </si>
+  <si>
+    <t>dmg-mla-17.jpg</t>
+  </si>
+  <si>
+    <t>a01082.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j.jpg</t>
+  </si>
+  <si>
+    <t>a01084.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-18.jpg</t>
+  </si>
+  <si>
+    <t>a01086.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-19.jpg</t>
+  </si>
+  <si>
+    <t>a01088.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-20.jpg</t>
+  </si>
+  <si>
+    <t>a01090.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-21.jpg</t>
+  </si>
+  <si>
+    <t>a01092.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-22.jpg</t>
+  </si>
+  <si>
+    <t>a01094.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-23.jpg</t>
+  </si>
+  <si>
+    <t>a01096.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-24.jpg</t>
+  </si>
+  <si>
+    <t>a01098.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-25.jpg</t>
+  </si>
+  <si>
+    <t>a01100.jpg</t>
+  </si>
+  <si>
+    <t>dmg-l6j-26.jpg</t>
+  </si>
+  <si>
+    <t>a01102.jpg</t>
+  </si>
+  <si>
+    <t>dmg-vua.jpg</t>
+  </si>
+  <si>
+    <t>a01104.jpg</t>
+  </si>
+  <si>
+    <t>dmg-vua-27.jpg</t>
+  </si>
+  <si>
+    <t>a01106.jpg</t>
+  </si>
+  <si>
+    <t>dmg-vua-28.jpg</t>
+  </si>
+  <si>
+    <t>a01108.jpg</t>
+  </si>
+  <si>
+    <t>dmg-vua-29.jpg</t>
+  </si>
+  <si>
+    <t>a01110.jpg</t>
+  </si>
+  <si>
+    <t>dmg-vua-30.jpg</t>
+  </si>
+  <si>
+    <t>a01112.jpg</t>
+  </si>
+  <si>
+    <t>dmg-vua-31.jpg</t>
+  </si>
+  <si>
+    <t>a01114.jpg</t>
+  </si>
+  <si>
+    <t>dmg-vua-32.jpg</t>
+  </si>
+  <si>
+    <t>a01116.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ap2j-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01118.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ap2j-jpn-33.jpg</t>
+  </si>
+  <si>
+    <t>a01120.jpg</t>
+  </si>
+  <si>
+    <t>dmg-agaj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01122.jpg</t>
+  </si>
+  <si>
+    <t>dmg-agij-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01124.jpg</t>
+  </si>
+  <si>
+    <t>dmg-wja.jpg</t>
+  </si>
+  <si>
+    <t>a01126.jpg</t>
+  </si>
+  <si>
+    <t>dmg-wja-34.jpg</t>
+  </si>
+  <si>
+    <t>a01128.jpg</t>
+  </si>
+  <si>
+    <t>dmg-wja-35.jpg</t>
+  </si>
+  <si>
+    <t>a01130.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aw2j-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01132.jpg</t>
+  </si>
+  <si>
+    <t>dmg-kyj.jpg</t>
+  </si>
+  <si>
+    <t>a01134.jpg</t>
+  </si>
+  <si>
+    <t>dmg-akbj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01136.jpg</t>
+  </si>
+  <si>
+    <t>dmg-akbj-jpn-36.jpg</t>
+  </si>
+  <si>
+    <t>a01138.jpg</t>
+  </si>
+  <si>
+    <t>dmg-akbj-jpn-37.jpg</t>
+  </si>
+  <si>
+    <t>a01140.jpg</t>
+  </si>
+  <si>
+    <t>dmg-akbj-jpn-38.jpg</t>
+  </si>
+  <si>
+    <t>a01142.jpg</t>
+  </si>
+  <si>
+    <t>dmg-k9j.jpg</t>
+  </si>
+  <si>
+    <t>a01144.jpg</t>
+  </si>
+  <si>
+    <t>dmg-yoj.jpg</t>
+  </si>
+  <si>
+    <t>a01146.jpg</t>
+  </si>
+  <si>
+    <t>dmg-yoj-39.jpg</t>
+  </si>
+  <si>
+    <t>a01148.jpg</t>
+  </si>
+  <si>
+    <t>dmg-yoj-40.jpg</t>
+  </si>
+  <si>
+    <t>a01150.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apsj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01152.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apsj-jpn-41.jpg</t>
+  </si>
+  <si>
+    <t>a01154.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apsj-jpn-42.jpg</t>
+  </si>
+  <si>
+    <t>a01156.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apsj-jpn-43.jpg</t>
+  </si>
+  <si>
+    <t>a01158.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apsj-jpn-44.jpg</t>
+  </si>
+  <si>
+    <t>a01160.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apaj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01162.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apaj-jpn-45.jpg</t>
+  </si>
+  <si>
+    <t>a01164.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apaj-jpn-46.jpg</t>
+  </si>
+  <si>
+    <t>a01166.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apaj-jpn-47.jpg</t>
+  </si>
+  <si>
+    <t>a01168.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apej-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01170.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apej-jpn-48.jpg</t>
+  </si>
+  <si>
+    <t>a01172.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apej-jpn-49.jpg</t>
+  </si>
+  <si>
+    <t>a01174.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apej-jpn-50.jpg</t>
+  </si>
+  <si>
+    <t>a01176.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01178.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-51.jpg</t>
+  </si>
+  <si>
+    <t>a01180.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-52.jpg</t>
+  </si>
+  <si>
+    <t>a01182.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-53.jpg</t>
+  </si>
+  <si>
+    <t>a01184.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-54.jpg</t>
+  </si>
+  <si>
+    <t>a01186.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-55.jpg</t>
+  </si>
+  <si>
+    <t>a01188.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-56.jpg</t>
+  </si>
+  <si>
+    <t>a01190.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-57.jpg</t>
+  </si>
+  <si>
+    <t>a01192.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-58.jpg</t>
+  </si>
+  <si>
+    <t>a01194.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-59.jpg</t>
+  </si>
+  <si>
+    <t>a01196.jpg</t>
+  </si>
+  <si>
+    <t>dmg-apbj-jpn-60.jpg</t>
+  </si>
+  <si>
+    <t>a01198.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aaxj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01200.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aaxj-jpn-61.jpg</t>
+  </si>
+  <si>
+    <t>a01202.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aaxj-jpn-62.jpg</t>
+  </si>
+  <si>
+    <t>a01204.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aaxj-jpn-63.jpg</t>
+  </si>
+  <si>
+    <t>a01206.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aaxj-jpn-64.jpg</t>
+  </si>
+  <si>
+    <t>a01208.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aaxj-jpn-65.jpg</t>
+  </si>
+  <si>
+    <t>a01210.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aauj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01212.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aauj-jpn-66.jpg</t>
+  </si>
+  <si>
+    <t>a01214.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aauj-jpn-67.jpg</t>
+  </si>
+  <si>
+    <t>a01216.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aauj-jpn-68.jpg</t>
+  </si>
+  <si>
+    <t>a01218.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aauj-jpn-69.jpg</t>
+  </si>
+  <si>
+    <t>a01220.jpg</t>
+  </si>
+  <si>
+    <t>dmg-acxj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01222.jpg</t>
+  </si>
+  <si>
+    <t>dmg-acxj-jpn-70.jpg</t>
+  </si>
+  <si>
+    <t>a01224.jpg</t>
+  </si>
+  <si>
+    <t>dmg-acxj-jpn-71.jpg</t>
+  </si>
+  <si>
+    <t>a01226.jpg</t>
+  </si>
+  <si>
+    <t>dmg-acxj-jpn-72.jpg</t>
+  </si>
+  <si>
+    <t>a01228.jpg</t>
+  </si>
+  <si>
+    <t>dmg-acxj-jpn-73.jpg</t>
+  </si>
+  <si>
+    <t>a01230.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra.jpg</t>
+  </si>
+  <si>
+    <t>a01232.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra-74.jpg</t>
+  </si>
+  <si>
+    <t>a01234.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra-75.jpg</t>
+  </si>
+  <si>
+    <t>a01236.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra-76.jpg</t>
+  </si>
+  <si>
+    <t>a01238.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra-77.jpg</t>
+  </si>
+  <si>
+    <t>a01240.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra-78.jpg</t>
+  </si>
+  <si>
+    <t>a01242.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra-79.jpg</t>
+  </si>
+  <si>
+    <t>a01244.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra-80.jpg</t>
+  </si>
+  <si>
+    <t>a01246.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tra-81.jpg</t>
+  </si>
+  <si>
+    <t>a01248.jpg</t>
+  </si>
+  <si>
+    <t>dmg-atea-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01250.jpg</t>
+  </si>
+  <si>
+    <t>dmg-w2j.jpg</t>
+  </si>
+  <si>
+    <t>a01252.jpg</t>
+  </si>
+  <si>
+    <t>dmg-hba.jpg</t>
+  </si>
+  <si>
+    <t>a01254.jpg</t>
+  </si>
+  <si>
+    <t>dmg-eej.jpg</t>
+  </si>
+  <si>
+    <t>a01256.jpg</t>
+  </si>
+  <si>
+    <t>dmg-abcj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01258.jpg</t>
+  </si>
+  <si>
+    <t>dmg-adpj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01260.jpg</t>
+  </si>
+  <si>
+    <t>dmg-m3j.jpg</t>
+  </si>
+  <si>
+    <t>a01262.jpg</t>
+  </si>
+  <si>
+    <t>dmg-j3j.jpg</t>
+  </si>
+  <si>
+    <t>a01264.jpg</t>
+  </si>
+  <si>
+    <t>dmg-mfj.jpg</t>
+  </si>
+  <si>
+    <t>a01266.jpg</t>
+  </si>
+  <si>
+    <t>dmg-coj.jpg</t>
+  </si>
+  <si>
+    <t>a01268.jpg</t>
+  </si>
+  <si>
+    <t>dmg-coj-82.jpg</t>
+  </si>
+  <si>
+    <t>a01270.jpg</t>
+  </si>
+  <si>
+    <t>dmg-hjj.jpg</t>
+  </si>
+  <si>
+    <t>a01272.jpg</t>
+  </si>
+  <si>
+    <t>dmg-hjj-83.jpg</t>
+  </si>
+  <si>
+    <t>a01274.jpg</t>
+  </si>
+  <si>
+    <t>dmg-hjj-84.jpg</t>
+  </si>
+  <si>
+    <t>a01276.jpg</t>
+  </si>
+  <si>
+    <t>dmg-aqj.jpg</t>
+  </si>
+  <si>
+    <t>a01278.jpg</t>
+  </si>
+  <si>
+    <t>dmg-adbj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01280.jpg</t>
+  </si>
+  <si>
+    <t>dmg-az2j-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01282.jpg</t>
+  </si>
+  <si>
+    <t>dmg-uuj.jpg</t>
+  </si>
+  <si>
+    <t>a01284.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ugj.jpg</t>
+  </si>
+  <si>
+    <t>a01286.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ugj-85.jpg</t>
+  </si>
+  <si>
+    <t>a01288.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ugj-86.jpg</t>
+  </si>
+  <si>
+    <t>a01290.jpg</t>
+  </si>
+  <si>
+    <t>dmg-d6j.jpg</t>
+  </si>
+  <si>
+    <t>a01292.jpg</t>
+  </si>
+  <si>
+    <t>dmg-sdj.jpg</t>
+  </si>
+  <si>
+    <t>a01294.jpg</t>
+  </si>
+  <si>
+    <t>dmg-sdj-87.jpg</t>
+  </si>
+  <si>
+    <t>a01296.jpg</t>
+  </si>
+  <si>
+    <t>dmg-sdj-88.jpg</t>
+  </si>
+  <si>
+    <t>a01298.jpg</t>
+  </si>
+  <si>
+    <t>dmg-lhj.jpg</t>
+  </si>
+  <si>
+    <t>a01300.jpg</t>
+  </si>
+  <si>
+    <t>dmg-lhj-89.jpg</t>
+  </si>
+  <si>
+    <t>a01302.jpg</t>
+  </si>
+  <si>
+    <t>dmg-xrj.jpg</t>
+  </si>
+  <si>
+    <t>a01304.jpg</t>
+  </si>
+  <si>
+    <t>dmg-t5j.jpg</t>
+  </si>
+  <si>
+    <t>a01306.jpg</t>
+  </si>
+  <si>
+    <t>dmg-a4bj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01308.jpg</t>
+  </si>
+  <si>
+    <t>dmg-qqj.jpg</t>
+  </si>
+  <si>
+    <t>a01310.jpg</t>
+  </si>
+  <si>
+    <t>dmg-qqj-90.jpg</t>
+  </si>
+  <si>
+    <t>a01312.jpg</t>
+  </si>
+  <si>
+    <t>dmg-qqj-91.jpg</t>
+  </si>
+  <si>
+    <t>a01314.jpg</t>
+  </si>
+  <si>
+    <t>dmg-gwj.jpg</t>
+  </si>
+  <si>
+    <t>a01316.jpg</t>
+  </si>
+  <si>
+    <t>dmg-gwj-92.jpg</t>
+  </si>
+  <si>
+    <t>a01318.jpg</t>
+  </si>
+  <si>
+    <t>dmg-cga.jpg</t>
+  </si>
+  <si>
+    <t>a01320.jpg</t>
+  </si>
+  <si>
+    <t>dmg-cga-93.jpg</t>
+  </si>
+  <si>
+    <t>a01322.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tbj.jpg</t>
+  </si>
+  <si>
+    <t>a01324.jpg</t>
+  </si>
+  <si>
+    <t>dmg-otj.jpg</t>
+  </si>
+  <si>
+    <t>a01326.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ada.jpg</t>
+  </si>
+  <si>
+    <t>a01328.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tvj.jpg</t>
+  </si>
+  <si>
+    <t>a01330.jpg</t>
+  </si>
+  <si>
+    <t>dmg-amoj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01332.jpg</t>
+  </si>
+  <si>
+    <t>dmg-amoj-jpn-94.jpg</t>
+  </si>
+  <si>
+    <t>a01334.jpg</t>
+  </si>
+  <si>
+    <t>dmg-soj.jpg</t>
+  </si>
+  <si>
+    <t>a01336.jpg</t>
+  </si>
+  <si>
+    <t>dmg-plj.jpg</t>
+  </si>
+  <si>
+    <t>a01338.jpg</t>
+  </si>
+  <si>
+    <t>dmg-asj.jpg</t>
+  </si>
+  <si>
+    <t>a01340.jpg</t>
+  </si>
+  <si>
+    <t>dmg-atj.jpg</t>
+  </si>
+  <si>
+    <t>a01342.jpg</t>
+  </si>
+  <si>
+    <t>dmg-ajlj-jpn.jpg</t>
+  </si>
+  <si>
+    <t>a01344.jpg</t>
+  </si>
+  <si>
+    <t>dmg-tdj.jpg</t>
+  </si>
+  <si>
+    <t>a01346.jpg</t>
+  </si>
+  <si>
+    <t>dmg-fij.jpg</t>
+  </si>
+  <si>
+    <t>a01348.jpg</t>
+  </si>
+  <si>
+    <t>dmg-qxa.jpg</t>
+  </si>
+  <si>
+    <t>a01350.jpg</t>
+  </si>
+  <si>
+    <t>dmg-awa.jpg</t>
+  </si>
+  <si>
+    <t>a01352.jpg</t>
+  </si>
+  <si>
+    <t>dmg-awa-95.jpg</t>
+  </si>
+  <si>
+    <t>a01354.jpg</t>
+  </si>
+  <si>
+    <t>dmg-qrj.jpg</t>
+  </si>
+  <si>
+    <t>a01356.jpg</t>
+  </si>
+  <si>
+    <t>dmg-qrj-96.jpg</t>
+  </si>
+  <si>
+    <t>a01358.jpg</t>
+  </si>
+  <si>
+    <t>dmg-nma.jpg</t>
+  </si>
+  <si>
+    <t>a01360.jpg</t>
+  </si>
+  <si>
+    <t>dmg-nma-97.jpg</t>
+  </si>
+  <si>
+    <t>a01362.jpg</t>
+  </si>
+  <si>
+    <t>dmg-nma-98.jpg</t>
+  </si>
+  <si>
+    <t>a01364.jpg</t>
+  </si>
+  <si>
+    <t>dmg-rea.jpg</t>
+  </si>
+  <si>
+    <t>a01366.jpg</t>
+  </si>
+  <si>
+    <t>dmg-bra.jpg</t>
+  </si>
+  <si>
+    <t>a01368.jpg</t>
+  </si>
+  <si>
+    <t>dmg-hqj.jpg</t>
+  </si>
+  <si>
+    <t>a01370.jpg</t>
+  </si>
+  <si>
+    <t>dmg-dha.jpg</t>
+  </si>
   <si>
     <t>a01372.jpg</t>
   </si>
   <si>
-    <t>agb-fsmj-jpn.jpg</t>
+    <t>dmg-mta.jpg</t>
   </si>
   <si>
     <t>a01374.jpg</t>
   </si>
   <si>
-    <t>agb-axvj-jpn.jpg</t>
+    <t>dmg-asfj-jpn.jpg</t>
   </si>
   <si>
     <t>a01376.jpg</t>
   </si>
   <si>
+    <t>dmg-x4j.jpg</t>
+  </si>
+  <si>
     <t>a01378.jpg</t>
   </si>
   <si>
-    <t>agb-bprj-jpn.jpg</t>
+    <t>dmg-x4j-99.jpg</t>
   </si>
   <si>
     <t>a01380.jpg</t>
   </si>
   <si>
-    <t>agb-axpj-jpn.jpg</t>
+    <t>dmg-x3j.jpg</t>
   </si>
   <si>
     <t>a01382.jpg</t>
   </si>
   <si>
+    <t>dmg-x3j-100.jpg</t>
+  </si>
+  <si>
     <t>a01384.jpg</t>
   </si>
   <si>
-    <t>agb-b4bj-jpn.jpg</t>
+    <t>dmg-chj.jpg</t>
   </si>
   <si>
     <t>a01386.jpg</t>
   </si>
   <si>
-    <t>agb-a7kj-jpn.jpg</t>
+    <t>dmg-kuj.jpg</t>
   </si>
   <si>
     <t>a01388.jpg</t>
   </si>
   <si>
-    <t>agb-bsbj-jpn.jpg</t>
+    <t>dmg-ncj.jpg</t>
   </si>
   <si>
     <t>a01390.jpg</t>
   </si>
   <si>
-    <t>agb-asoj-jpn.jpg</t>
+    <t>dmg-ncj-101.jpg</t>
   </si>
   <si>
     <t>a01392.jpg</t>
   </si>
   <si>
-    <t>agb-brbj-jpn.jpg</t>
+    <t>dmg-ncj-102.jpg</t>
   </si>
   <si>
     <t>a01394.jpg</t>
   </si>
   <si>
-    <t>agb-br5j-jpn.jpg</t>
+    <t>dmg-ncj-103.jpg</t>
   </si>
   <si>
     <t>a01396.jpg</t>
   </si>
   <si>
+    <t>dmg-duj.jpg</t>
+  </si>
+  <si>
     <t>a01398.jpg</t>
   </si>
   <si>
-    <t>agb-a3gj-jpn.jpg</t>
+    <t>dmg-afdj-jpn.jpg</t>
   </si>
   <si>
     <t>a01400.jpg</t>
   </si>
   <si>
-    <t>agb-a9lj-jpn.jpg</t>
+    <t>dmg-ymj.jpg</t>
   </si>
   <si>
     <t>a01402.jpg</t>
   </si>
   <si>
-    <t>agb-ausj-jpn.jpg</t>
+    <t>dmg-ngj.jpg</t>
   </si>
   <si>
     <t>a01404.jpg</t>
   </si>
   <si>
-    <t>agb-a4gj-jpn.jpg</t>
+    <t>dmg-cpa.jpg</t>
   </si>
   <si>
     <t>a01406.jpg</t>
   </si>
   <si>
-    <t>agb-bnrj-jpn.jpg</t>
+    <t>dmg-mea.jpg</t>
   </si>
   <si>
     <t>a01408.jpg</t>
   </si>
   <si>
-    <t>agb-amtj-jpn.jpg</t>
+    <t>dmg-mea-104.jpg</t>
   </si>
   <si>
     <t>a01410.jpg</t>
   </si>
   <si>
-    <t>agb-arhj-jpn.jpg</t>
+    <t>dmg-mea-105.jpg</t>
   </si>
   <si>
     <t>a01412.jpg</t>
   </si>
   <si>
-    <t>agb-amuj-jpn.jpg</t>
+    <t>dmg-mea-106.jpg</t>
   </si>
   <si>
     <t>a01414.jpg</t>
   </si>
   <si>
-    <t>agb-bngj-jpn.jpg</t>
+    <t>dmg-dfj.jpg</t>
   </si>
   <si>
     <t>a01416.jpg</t>
   </si>
   <si>
-    <t>agb-azgj-jpn.jpg</t>
+    <t>dmg-cvj.jpg</t>
   </si>
   <si>
     <t>a01418.jpg</t>
   </si>
   <si>
-    <t>dmg-ataj-jpn.jpg</t>
+    <t>dmg-cwj.jpg</t>
   </si>
   <si>
     <t>a01420.jpg</t>
   </si>
   <si>
+    <t>dmg-zoj.jpg</t>
+  </si>
+  <si>
     <t>a01422.jpg</t>
   </si>
   <si>
+    <t>dmg-gcj.jpg</t>
+  </si>
+  <si>
     <t>a01424.jpg</t>
   </si>
   <si>
+    <t>dmg-t3j.jpg</t>
+  </si>
+  <si>
     <t>a01426.jpg</t>
   </si>
   <si>
-    <t>dmg-at3j-jpn.jpg</t>
+    <t>dmg-ag3j-jpn.jpg</t>
   </si>
   <si>
     <t>a01428.jpg</t>
   </si>
   <si>
+    <t>dmg-txj.jpg</t>
+  </si>
+  <si>
     <t>a01430.jpg</t>
   </si>
   <si>
+    <t>dmg-mma.jpg</t>
+  </si>
+  <si>
     <t>a01432.jpg</t>
   </si>
   <si>
+    <t>dmg-m2a.jpg</t>
+  </si>
+  <si>
     <t>a01434.jpg</t>
   </si>
   <si>
-    <t>dmg-ytj.jpg</t>
+    <t>dmg-amrj-jpn.jpg</t>
   </si>
   <si>
     <t>a01436.jpg</t>
   </si>
   <si>
+    <t>dmg-aywj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01438.jpg</t>
   </si>
   <si>
+    <t>dmg-pbj.jpg</t>
+  </si>
+  <si>
     <t>a01440.jpg</t>
   </si>
   <si>
-    <t>dmg-mla.jpg</t>
+    <t>dmg-hhj.jpg</t>
   </si>
   <si>
     <t>a01442.jpg</t>
   </si>
   <si>
+    <t>dmg-laj.jpg</t>
+  </si>
+  <si>
     <t>a01444.jpg</t>
   </si>
   <si>
+    <t>dmg-l2j.jpg</t>
+  </si>
+  <si>
     <t>a01446.jpg</t>
   </si>
   <si>
+    <t>dmg-gxj.jpg</t>
+  </si>
+  <si>
     <t>a01448.jpg</t>
   </si>
   <si>
+    <t>dmg-hej.jpg</t>
+  </si>
+  <si>
     <t>a01450.jpg</t>
   </si>
   <si>
+    <t>dmg-ffj.jpg</t>
+  </si>
+  <si>
     <t>a01452.jpg</t>
   </si>
   <si>
+    <t>dmg-a9yj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01454.jpg</t>
   </si>
   <si>
-    <t>dmg-l6j.jpg</t>
+    <t>dmg-wij.jpg</t>
   </si>
   <si>
     <t>a01456.jpg</t>
   </si>
   <si>
+    <t>dmg-w5j.jpg</t>
+  </si>
+  <si>
     <t>a01458.jpg</t>
   </si>
   <si>
+    <t>dmg-w6j.jpg</t>
+  </si>
+  <si>
     <t>a01460.jpg</t>
   </si>
   <si>
+    <t>dmg-saj.jpg</t>
+  </si>
+  <si>
     <t>a01462.jpg</t>
   </si>
   <si>
+    <t>dmg-saj-107.jpg</t>
+  </si>
+  <si>
     <t>a01464.jpg</t>
   </si>
   <si>
+    <t>dmg-s2j.jpg</t>
+  </si>
+  <si>
     <t>a01466.jpg</t>
   </si>
   <si>
+    <t>dmg-s2j-108.jpg</t>
+  </si>
+  <si>
     <t>a01468.jpg</t>
   </si>
   <si>
+    <t>dmg-s2j-109.jpg</t>
+  </si>
+  <si>
     <t>a01470.jpg</t>
   </si>
   <si>
+    <t>dmg-s2j-110.jpg</t>
+  </si>
+  <si>
     <t>a01472.jpg</t>
   </si>
   <si>
+    <t>dmg-osj.jpg</t>
+  </si>
+  <si>
     <t>a01474.jpg</t>
   </si>
   <si>
-    <t>dmg-vua.jpg</t>
+    <t>dmg-osj-111.jpg</t>
   </si>
   <si>
     <t>a01476.jpg</t>
   </si>
   <si>
+    <t>dmg-osj-112.jpg</t>
+  </si>
+  <si>
     <t>a01478.jpg</t>
   </si>
   <si>
+    <t>dmg-zlj.jpg</t>
+  </si>
+  <si>
     <t>a01480.jpg</t>
   </si>
   <si>
+    <t>dmg-azlj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01482.jpg</t>
   </si>
   <si>
+    <t>dmg-azlj-jpn-113.jpg</t>
+  </si>
+  <si>
     <t>a01484.jpg</t>
   </si>
   <si>
+    <t>dmg-amyj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01486.jpg</t>
   </si>
   <si>
+    <t>dmg-amyj-jpn-114.jpg</t>
+  </si>
+  <si>
     <t>a01488.jpg</t>
   </si>
   <si>
-    <t>dmg-ap2j-jpn.jpg</t>
+    <t>dmg-a8cj-jpn.jpg</t>
   </si>
   <si>
     <t>a01490.jpg</t>
   </si>
   <si>
+    <t>dmg-aedj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01492.jpg</t>
   </si>
   <si>
-    <t>dmg-agaj-jpn.jpg</t>
+    <t>dmg-bqlj-jpn.jpg</t>
   </si>
   <si>
     <t>a01494.jpg</t>
   </si>
   <si>
-    <t>dmg-agij-jpn.jpg</t>
+    <t>dmg-bhnj-jpn.jpg</t>
   </si>
   <si>
     <t>a01496.jpg</t>
   </si>
   <si>
-    <t>dmg-wja.jpg</t>
+    <t>dmg-ahhj-jpn.jpg</t>
   </si>
   <si>
     <t>a01498.jpg</t>
   </si>
   <si>
+    <t>dmg-abdj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01500.jpg</t>
   </si>
   <si>
+    <t>dmg-am7j-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01502.jpg</t>
   </si>
   <si>
-    <t>dmg-aw2j-jpn.jpg</t>
+    <t>dmg-am7j-jpn-115.jpg</t>
   </si>
   <si>
     <t>a01504.jpg</t>
   </si>
   <si>
-    <t>dmg-kyj.jpg</t>
+    <t>dmg-am7j-jpn-116.jpg</t>
   </si>
   <si>
     <t>a01506.jpg</t>
   </si>
   <si>
-    <t>dmg-akbj-jpn.jpg</t>
+    <t>dmg-am7j-jpn-117.jpg</t>
   </si>
   <si>
     <t>a01508.jpg</t>
   </si>
   <si>
+    <t>dmg-am7j-jpn-118.jpg</t>
+  </si>
+  <si>
     <t>a01510.jpg</t>
   </si>
   <si>
+    <t>cgb-bm8j-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01512.jpg</t>
   </si>
   <si>
+    <t>cgb-bm8j-jpn-119.jpg</t>
+  </si>
+  <si>
     <t>a01514.jpg</t>
   </si>
   <si>
-    <t>dmg-k9j.jpg</t>
+    <t>cgb-az7j-jpn.jpg</t>
   </si>
   <si>
     <t>a01516.jpg</t>
   </si>
   <si>
-    <t>dmg-yoj.jpg</t>
+    <t>cgb-az7j-jpn-120.jpg</t>
   </si>
   <si>
     <t>a01518.jpg</t>
   </si>
   <si>
+    <t>cgb-az8j-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01520.jpg</t>
   </si>
   <si>
+    <t>cgb-bd3j-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01522.jpg</t>
   </si>
   <si>
-    <t>dmg-apsj-jpn.jpg</t>
+    <t>cgb-bd3j-jpn-121.jpg</t>
   </si>
   <si>
     <t>a01524.jpg</t>
   </si>
   <si>
+    <t>cgb-b32j-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01526.jpg</t>
   </si>
   <si>
+    <t>cgb-b3pj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01528.jpg</t>
   </si>
   <si>
+    <t>cgb-bhhj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01530.jpg</t>
   </si>
   <si>
+    <t>cgb-bhhj-jpn-122.jpg</t>
+  </si>
+  <si>
     <t>a01532.jpg</t>
   </si>
   <si>
-    <t>dmg-apaj-jpn.jpg</t>
+    <t>cgb-a2qj-jpn.jpg</t>
   </si>
   <si>
     <t>a01534.jpg</t>
   </si>
   <si>
+    <t>cgb-b22j-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01536.jpg</t>
   </si>
   <si>
+    <t>cgb-b3dj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01538.jpg</t>
   </si>
   <si>
+    <t>cgb-bxtj-jpn.jpg</t>
+  </si>
+  <si>
     <t>a01540.jpg</t>
   </si>
   <si>
-    <t>dmg-apej-jpn.jpg</t>
+    <t>cgb-bxtj-jpn-123.jpg</t>
   </si>
   <si>
     <t>a01542.jpg</t>
   </si>
   <si>
+    <t>cgb-bxtj-jpn-124.jpg</t>
+  </si>
+  <si>
     <t>a01544.jpg</t>
   </si>
   <si>
+    <t>cgb-bxtj-jpn-125.jpg</t>
+  </si>
+  <si>
     <t>a01546.jpg</t>
   </si>
   <si>
+    <t>mgb-006-cp.jpg</t>
+  </si>
+  <si>
     <t>a01548.jpg</t>
   </si>
   <si>
-    <t>dmg-apbj-jpn.jpg</t>
+    <t>dmg-mmsa-jpn.jpg</t>
   </si>
   <si>
     <t>a01551.jpg</t>
   </si>
   <si>
+    <t>dmg-mmsa-jpn-126.jpg</t>
+  </si>
+  <si>
     <t>a01554.jpg</t>
   </si>
   <si>
+    <t>dmg-mmsa-jpn-127.jpg</t>
+  </si>
+  <si>
     <t>a01557.jpg</t>
   </si>
   <si>
+    <t>dmg-apbj-jpn-128.jpg</t>
+  </si>
+  <si>
     <t>a01560.jpg</t>
   </si>
   <si>
+    <t>dmg-apsj-jpn-129.jpg</t>
+  </si>
+  <si>
     <t>a01563.jpg</t>
   </si>
   <si>
+    <t>dmg-apaj-jpn-130.jpg</t>
+  </si>
+  <si>
     <t>a01566.jpg</t>
   </si>
   <si>
+    <t>dmg-mla-131.jpg</t>
+  </si>
+  <si>
     <t>a01569.jpg</t>
   </si>
   <si>
+    <t>dmg-l6j-132.jpg</t>
+  </si>
+  <si>
     <t>a01572.jpg</t>
   </si>
   <si>
+    <t>dmg-l6j-133.jpg</t>
+  </si>
+  <si>
     <t>a01575.jpg</t>
   </si>
   <si>
+    <t>dmg-tra-134.jpg</t>
+  </si>
+  <si>
     <t>a01578.jpg</t>
   </si>
   <si>
+    <t>dmg-apaj-jpn-135.jpg</t>
+  </si>
+  <si>
     <t>a01581.jpg</t>
   </si>
   <si>
-    <t>dmg-aaxj-jpn.jpg</t>
+    <t>cgb-kkkj-jpn.jpg</t>
   </si>
 </sst>
 </file>
@@ -765,7 +2061,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -792,783 +2088,2271 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="B66" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="B67" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="B68" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="B71" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="B72" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="B74" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="B81" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="B82" t="s">
-        <v>117</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="B85" t="s">
-        <v>122</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="B86" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="B87" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="B90" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>129</v>
+        <v>180</v>
       </c>
       <c r="B91" t="s">
-        <v>127</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="B93" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>132</v>
+        <v>186</v>
       </c>
       <c r="B94" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>133</v>
+        <v>188</v>
       </c>
       <c r="B95" t="s">
-        <v>127</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>134</v>
+        <v>190</v>
       </c>
       <c r="B96" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="B97" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>136</v>
+        <v>194</v>
       </c>
       <c r="B98" t="s">
-        <v>127</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="B99" t="s">
-        <v>127</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>138</v>
+        <v>198</v>
       </c>
       <c r="B100" t="s">
-        <v>139</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>236</v>
+      </c>
+      <c r="B119" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>242</v>
+      </c>
+      <c r="B122" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>250</v>
+      </c>
+      <c r="B126" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>252</v>
+      </c>
+      <c r="B127" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>254</v>
+      </c>
+      <c r="B128" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>256</v>
+      </c>
+      <c r="B129" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>258</v>
+      </c>
+      <c r="B130" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>260</v>
+      </c>
+      <c r="B131" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>262</v>
+      </c>
+      <c r="B132" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>264</v>
+      </c>
+      <c r="B133" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>266</v>
+      </c>
+      <c r="B134" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>268</v>
+      </c>
+      <c r="B135" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>270</v>
+      </c>
+      <c r="B136" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>272</v>
+      </c>
+      <c r="B137" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>274</v>
+      </c>
+      <c r="B138" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>276</v>
+      </c>
+      <c r="B139" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>278</v>
+      </c>
+      <c r="B140" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>280</v>
+      </c>
+      <c r="B141" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>282</v>
+      </c>
+      <c r="B142" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>284</v>
+      </c>
+      <c r="B143" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>286</v>
+      </c>
+      <c r="B144" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>288</v>
+      </c>
+      <c r="B145" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>290</v>
+      </c>
+      <c r="B146" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>292</v>
+      </c>
+      <c r="B147" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>294</v>
+      </c>
+      <c r="B148" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>296</v>
+      </c>
+      <c r="B149" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>298</v>
+      </c>
+      <c r="B150" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>300</v>
+      </c>
+      <c r="B151" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>302</v>
+      </c>
+      <c r="B152" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>308</v>
+      </c>
+      <c r="B155" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>310</v>
+      </c>
+      <c r="B156" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>314</v>
+      </c>
+      <c r="B158" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>316</v>
+      </c>
+      <c r="B159" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>318</v>
+      </c>
+      <c r="B160" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>320</v>
+      </c>
+      <c r="B161" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>322</v>
+      </c>
+      <c r="B162" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>324</v>
+      </c>
+      <c r="B163" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>326</v>
+      </c>
+      <c r="B164" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>328</v>
+      </c>
+      <c r="B165" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>332</v>
+      </c>
+      <c r="B167" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>334</v>
+      </c>
+      <c r="B168" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>336</v>
+      </c>
+      <c r="B169" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>338</v>
+      </c>
+      <c r="B170" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>340</v>
+      </c>
+      <c r="B171" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>342</v>
+      </c>
+      <c r="B172" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>346</v>
+      </c>
+      <c r="B174" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>348</v>
+      </c>
+      <c r="B175" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>352</v>
+      </c>
+      <c r="B177" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>354</v>
+      </c>
+      <c r="B178" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>356</v>
+      </c>
+      <c r="B179" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>358</v>
+      </c>
+      <c r="B180" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>360</v>
+      </c>
+      <c r="B181" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>362</v>
+      </c>
+      <c r="B182" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>364</v>
+      </c>
+      <c r="B183" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>366</v>
+      </c>
+      <c r="B184" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>368</v>
+      </c>
+      <c r="B185" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>370</v>
+      </c>
+      <c r="B186" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>372</v>
+      </c>
+      <c r="B187" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>374</v>
+      </c>
+      <c r="B188" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>376</v>
+      </c>
+      <c r="B189" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>378</v>
+      </c>
+      <c r="B190" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>380</v>
+      </c>
+      <c r="B191" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>382</v>
+      </c>
+      <c r="B192" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>384</v>
+      </c>
+      <c r="B193" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>386</v>
+      </c>
+      <c r="B194" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>388</v>
+      </c>
+      <c r="B195" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>390</v>
+      </c>
+      <c r="B196" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>392</v>
+      </c>
+      <c r="B197" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>394</v>
+      </c>
+      <c r="B198" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>396</v>
+      </c>
+      <c r="B199" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>398</v>
+      </c>
+      <c r="B200" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>400</v>
+      </c>
+      <c r="B201" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>402</v>
+      </c>
+      <c r="B202" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>404</v>
+      </c>
+      <c r="B203" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>406</v>
+      </c>
+      <c r="B204" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>408</v>
+      </c>
+      <c r="B205" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>410</v>
+      </c>
+      <c r="B206" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>412</v>
+      </c>
+      <c r="B207" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>414</v>
+      </c>
+      <c r="B208" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>416</v>
+      </c>
+      <c r="B209" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>418</v>
+      </c>
+      <c r="B210" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>420</v>
+      </c>
+      <c r="B211" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>422</v>
+      </c>
+      <c r="B212" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>424</v>
+      </c>
+      <c r="B213" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>426</v>
+      </c>
+      <c r="B214" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>428</v>
+      </c>
+      <c r="B215" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>430</v>
+      </c>
+      <c r="B216" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>432</v>
+      </c>
+      <c r="B217" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>434</v>
+      </c>
+      <c r="B218" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>436</v>
+      </c>
+      <c r="B219" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>438</v>
+      </c>
+      <c r="B220" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>440</v>
+      </c>
+      <c r="B221" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>442</v>
+      </c>
+      <c r="B222" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>444</v>
+      </c>
+      <c r="B223" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>446</v>
+      </c>
+      <c r="B224" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>448</v>
+      </c>
+      <c r="B225" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>450</v>
+      </c>
+      <c r="B226" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>452</v>
+      </c>
+      <c r="B227" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>454</v>
+      </c>
+      <c r="B228" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>456</v>
+      </c>
+      <c r="B229" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>458</v>
+      </c>
+      <c r="B230" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>460</v>
+      </c>
+      <c r="B231" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>462</v>
+      </c>
+      <c r="B232" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>464</v>
+      </c>
+      <c r="B233" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>466</v>
+      </c>
+      <c r="B234" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>468</v>
+      </c>
+      <c r="B235" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>470</v>
+      </c>
+      <c r="B236" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>472</v>
+      </c>
+      <c r="B237" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>474</v>
+      </c>
+      <c r="B238" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>476</v>
+      </c>
+      <c r="B239" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>478</v>
+      </c>
+      <c r="B240" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>480</v>
+      </c>
+      <c r="B241" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>482</v>
+      </c>
+      <c r="B242" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>484</v>
+      </c>
+      <c r="B243" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>486</v>
+      </c>
+      <c r="B244" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>488</v>
+      </c>
+      <c r="B245" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>490</v>
+      </c>
+      <c r="B246" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>492</v>
+      </c>
+      <c r="B247" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>494</v>
+      </c>
+      <c r="B248" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>496</v>
+      </c>
+      <c r="B249" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>498</v>
+      </c>
+      <c r="B250" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>500</v>
+      </c>
+      <c r="B251" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" t="s">
+        <v>502</v>
+      </c>
+      <c r="B252" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" t="s">
+        <v>504</v>
+      </c>
+      <c r="B253" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" t="s">
+        <v>506</v>
+      </c>
+      <c r="B254" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" t="s">
+        <v>508</v>
+      </c>
+      <c r="B255" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>510</v>
+      </c>
+      <c r="B256" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>512</v>
+      </c>
+      <c r="B257" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>514</v>
+      </c>
+      <c r="B258" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>516</v>
+      </c>
+      <c r="B259" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>518</v>
+      </c>
+      <c r="B260" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>520</v>
+      </c>
+      <c r="B261" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>522</v>
+      </c>
+      <c r="B262" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>524</v>
+      </c>
+      <c r="B263" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>526</v>
+      </c>
+      <c r="B264" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" t="s">
+        <v>528</v>
+      </c>
+      <c r="B265" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266" t="s">
+        <v>530</v>
+      </c>
+      <c r="B266" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" t="s">
+        <v>532</v>
+      </c>
+      <c r="B267" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268" t="s">
+        <v>534</v>
+      </c>
+      <c r="B268" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269" t="s">
+        <v>536</v>
+      </c>
+      <c r="B269" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270" t="s">
+        <v>538</v>
+      </c>
+      <c r="B270" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" t="s">
+        <v>540</v>
+      </c>
+      <c r="B271" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="A272" t="s">
+        <v>542</v>
+      </c>
+      <c r="B272" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273" t="s">
+        <v>544</v>
+      </c>
+      <c r="B273" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>546</v>
+      </c>
+      <c r="B274" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
+        <v>548</v>
+      </c>
+      <c r="B275" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
+        <v>550</v>
+      </c>
+      <c r="B276" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>552</v>
+      </c>
+      <c r="B277" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>554</v>
+      </c>
+      <c r="B278" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279" t="s">
+        <v>556</v>
+      </c>
+      <c r="B279" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280" t="s">
+        <v>558</v>
+      </c>
+      <c r="B280" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281" t="s">
+        <v>560</v>
+      </c>
+      <c r="B281" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282" t="s">
+        <v>562</v>
+      </c>
+      <c r="B282" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283" t="s">
+        <v>564</v>
+      </c>
+      <c r="B283" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="A284" t="s">
+        <v>566</v>
+      </c>
+      <c r="B284" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285" t="s">
+        <v>568</v>
+      </c>
+      <c r="B285" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" t="s">
+        <v>570</v>
+      </c>
+      <c r="B286" t="s">
+        <v>571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>